<commit_message>
add the article effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Article.xlsx
+++ b/ConfigData/Xlsx/Article.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>描述</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>图标</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -52,21 +48,76 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Descript</t>
+    <t>增加LP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddLp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddMp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加PP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddPp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mix1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mix2</t>
+  </si>
+  <si>
+    <t>mix3</t>
+  </si>
+  <si>
+    <t>LP+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PP+2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特效</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Icon</t>
-  </si>
-  <si>
-    <t>快速</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>每次移动消耗食物-1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mental1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowflash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>redflash</t>
+  </si>
+  <si>
+    <t>blueflash</t>
   </si>
 </sst>
 </file>
@@ -804,31 +855,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1055,16 +1086,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:D4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:D4"/>
-  <sortState ref="A4:D4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:G6"/>
+  <sortState ref="A4:G4">
     <sortCondition ref="A3:A4"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="7">
     <tableColumn id="1" name="Id" dataDxfId="4"/>
     <tableColumn id="2" name="Name" dataDxfId="3"/>
-    <tableColumn id="3" name="Descript" dataDxfId="2"/>
-    <tableColumn id="9" name="Icon" dataDxfId="1"/>
+    <tableColumn id="4" name="AddLp"/>
+    <tableColumn id="5" name="AddMp"/>
+    <tableColumn id="6" name="AddPp"/>
+    <tableColumn id="7" name="Effect"/>
+    <tableColumn id="9" name="Icon" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1391,24 +1425,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.875" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" customWidth="1"/>
+    <col min="3" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1416,59 +1451,128 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>58000001</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>58000002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>58000003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:D4">
-    <cfRule type="containsBlanks" dxfId="0" priority="17">
+  <conditionalFormatting sqref="B4:E6 G4:G6">
+    <cfRule type="containsBlanks" dxfId="1" priority="18">
       <formula>LEN(TRIM(B4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F6">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix some fight bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Article.xlsx
+++ b/ConfigData/Xlsx/Article.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2B9CB0FF-1440-4495-B423-A70248C71DB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Article" sheetId="1" r:id="rId1"/>
@@ -94,20 +95,22 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>特效</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blueflash</t>
+  </si>
+  <si>
     <t>PP+2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>特效</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Effect</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>yellowflash</t>
@@ -115,15 +118,13 @@
   </si>
   <si>
     <t>redflash</t>
-  </si>
-  <si>
-    <t>blueflash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,20 +849,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1000,75 +987,23 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -1086,19 +1021,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:G6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:G6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:G6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:G4">
     <sortCondition ref="A3:A4"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" name="Name" dataDxfId="3"/>
-    <tableColumn id="4" name="AddLp"/>
-    <tableColumn id="5" name="AddMp"/>
-    <tableColumn id="6" name="AddPp"/>
-    <tableColumn id="7" name="Effect"/>
-    <tableColumn id="9" name="Icon" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="AddLp"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AddMp"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="AddPp"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effect"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Icon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,7 +1047,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1424,14 +1359,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1460,7 +1395,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>2</v>
@@ -1506,10 +1441,10 @@
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1517,13 +1452,13 @@
         <v>58000001</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1534,9 +1469,9 @@
         <v>58000002</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
@@ -1551,9 +1486,9 @@
         <v>58000003</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="C6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
@@ -1566,12 +1501,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B4:E6 G4:G6">
-    <cfRule type="containsBlanks" dxfId="1" priority="18">
+    <cfRule type="containsBlanks" dxfId="7" priority="18">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
draw random cell for random article
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Article.xlsx
+++ b/ConfigData/Xlsx/Article.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2B9CB0FF-1440-4495-B423-A70248C71DB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Article" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>序列</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -118,14 +117,26 @@
   </si>
   <si>
     <t>redflash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>分组</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +312,13 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -776,7 +794,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -800,6 +818,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -847,7 +871,49 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -987,23 +1053,75 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFB31D96"/>
       <color rgb="FFF577AD"/>
@@ -1021,19 +1139,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:G6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3" headerRowCellStyle="百分比">
-  <autoFilter ref="A3:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:G4">
-    <sortCondition ref="A3:A4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="百分比">
+  <autoFilter ref="A3:H9"/>
+  <sortState ref="A4:H9">
+    <sortCondition ref="A3:A9"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="AddLp"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="AddMp"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="AddPp"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effect"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Icon" dataDxfId="0"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Id" dataDxfId="8"/>
+    <tableColumn id="2" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" name="Group"/>
+    <tableColumn id="4" name="AddLp"/>
+    <tableColumn id="5" name="AddMp"/>
+    <tableColumn id="6" name="AddPp"/>
+    <tableColumn id="7" name="Effect"/>
+    <tableColumn id="9" name="Icon" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,7 +1166,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1359,8 +1478,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -1373,12 +1492,13 @@
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.125" customWidth="1"/>
-    <col min="3" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" customWidth="1"/>
+    <col min="4" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1386,22 +1506,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1409,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1417,14 +1540,17 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1432,56 +1558,65 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>58000001</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>58000002</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="E5">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>58000003</v>
       </c>
@@ -1489,25 +1624,98 @@
         <v>17</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="8">
+        <v>58000101</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>58000102</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>58000103</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="B4:E6 G4:G6">
-    <cfRule type="containsBlanks" dxfId="7" priority="18">
+  <conditionalFormatting sqref="B4:F9 H4:H9">
+    <cfRule type="containsBlanks" dxfId="5" priority="20">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:F6">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
-      <formula>LEN(TRIM(F4))=0</formula>
+  <conditionalFormatting sqref="G4:G9">
+    <cfRule type="containsBlanks" dxfId="4" priority="3">
+      <formula>LEN(TRIM(G4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:F9 H7:H9">
+    <cfRule type="containsBlanks" dxfId="3" priority="2">
+      <formula>LEN(TRIM(B7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G9">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(G7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>